<commit_message>
modified:   aula037/main.py 	new file:   aula037/reading.py 	modified:   aula037/workbook.xlsx
</commit_message>
<xml_diff>
--- a/secao_4/aula037/workbook.xlsx
+++ b/secao_4/aula037/workbook.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Minha Planilha" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,7 +448,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>6.8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -474,7 +474,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">

</xml_diff>